<commit_message>
timedelta and 1904 datetime system
</commit_message>
<xml_diff>
--- a/tests/date.xlsx
+++ b/tests/date.xlsx
@@ -21,9 +21,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="[hh]:mm:ss"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -90,12 +91,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -112,14 +121,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A:A"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -131,7 +140,7 @@
       <c r="A1" s="1" t="n">
         <v>44197</v>
       </c>
-      <c r="B1" s="0" t="n">
+      <c r="B1" s="2" t="n">
         <v>15</v>
       </c>
     </row>
@@ -139,17 +148,25 @@
       <c r="A2" s="1" t="n">
         <v>44198</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="2" t="n">
         <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="n">
+        <v>10.6320601851852</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>